<commit_message>
#1326 integration test added
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/IntegrationSample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/IntegrationSample1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdelRodriguez\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.R.Tests\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0932E670-86BB-4D6D-B572-6C1A329030F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D00D0C-162C-4DDC-8FD2-3615B040848C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2208" yWindow="1248" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>time  [h]</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>SD [mg/l]</t>
+  </si>
+  <si>
+    <t>Molecular Weight</t>
   </si>
 </sst>
 </file>
@@ -386,17 +389,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="12.3125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -406,8 +411,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -417,8 +425,11 @@
       <c r="C2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>0.24454149999999999</v>
       </c>
@@ -428,8 +439,11 @@
       <c r="C3" s="2">
         <v>6.9781999999999997E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>0.50655019999999995</v>
       </c>
@@ -439,8 +453,11 @@
       <c r="C4" s="2">
         <v>0.16947039999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
         <v>0.76855899999999999</v>
       </c>
@@ -450,8 +467,11 @@
       <c r="C5" s="2">
         <v>0.1919004</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>0.9956332</v>
       </c>
@@ -461,8 +481,11 @@
       <c r="C6" s="2">
         <v>0.16697809999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
         <v>1.2576419999999999</v>
       </c>
@@ -472,8 +495,11 @@
       <c r="C7" s="2">
         <v>0.13457939999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>1.502183</v>
       </c>
@@ -483,8 +509,11 @@
       <c r="C8" s="2">
         <v>0.12710279999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>1.764192</v>
       </c>
@@ -494,8 +523,11 @@
       <c r="C9" s="2">
         <v>0.12959490000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
         <v>2.008734</v>
       </c>
@@ -505,8 +537,11 @@
       <c r="C10" s="2">
         <v>0.1246106</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>3.0043669999999998</v>
       </c>
@@ -516,8 +551,11 @@
       <c r="C11" s="2">
         <v>0.1246106</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>4</v>
       </c>
@@ -527,8 +565,11 @@
       <c r="C12" s="2">
         <v>7.9750799999999997E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>6.0087339999999996</v>
       </c>
@@ -538,8 +579,11 @@
       <c r="C13" s="2">
         <v>4.2367599999999998E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>8</v>
       </c>
@@ -549,8 +593,11 @@
       <c r="C14" s="2">
         <v>2.2429899999999999E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
         <v>12.017469999999999</v>
       </c>
@@ -559,6 +606,9 @@
       </c>
       <c r="C15" s="2">
         <v>9.9688499999999996E-3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#1326 integration test added (#1331)
* #1326 integration test added

* red test corrected, not working tests removed
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/IntegrationSample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/IntegrationSample1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdelRodriguez\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.R.Tests\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0932E670-86BB-4D6D-B572-6C1A329030F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D00D0C-162C-4DDC-8FD2-3615B040848C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2208" yWindow="1248" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>time  [h]</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>SD [mg/l]</t>
+  </si>
+  <si>
+    <t>Molecular Weight</t>
   </si>
 </sst>
 </file>
@@ -386,17 +389,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="12.3125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -406,8 +411,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -417,8 +425,11 @@
       <c r="C2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>0.24454149999999999</v>
       </c>
@@ -428,8 +439,11 @@
       <c r="C3" s="2">
         <v>6.9781999999999997E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>0.50655019999999995</v>
       </c>
@@ -439,8 +453,11 @@
       <c r="C4" s="2">
         <v>0.16947039999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
         <v>0.76855899999999999</v>
       </c>
@@ -450,8 +467,11 @@
       <c r="C5" s="2">
         <v>0.1919004</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>0.9956332</v>
       </c>
@@ -461,8 +481,11 @@
       <c r="C6" s="2">
         <v>0.16697809999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
         <v>1.2576419999999999</v>
       </c>
@@ -472,8 +495,11 @@
       <c r="C7" s="2">
         <v>0.13457939999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>1.502183</v>
       </c>
@@ -483,8 +509,11 @@
       <c r="C8" s="2">
         <v>0.12710279999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>1.764192</v>
       </c>
@@ -494,8 +523,11 @@
       <c r="C9" s="2">
         <v>0.12959490000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
         <v>2.008734</v>
       </c>
@@ -505,8 +537,11 @@
       <c r="C10" s="2">
         <v>0.1246106</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>3.0043669999999998</v>
       </c>
@@ -516,8 +551,11 @@
       <c r="C11" s="2">
         <v>0.1246106</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>4</v>
       </c>
@@ -527,8 +565,11 @@
       <c r="C12" s="2">
         <v>7.9750799999999997E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>6.0087339999999996</v>
       </c>
@@ -538,8 +579,11 @@
       <c r="C13" s="2">
         <v>4.2367599999999998E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>8</v>
       </c>
@@ -549,8 +593,11 @@
       <c r="C14" s="2">
         <v>2.2429899999999999E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
         <v>12.017469999999999</v>
       </c>
@@ -559,6 +606,9 @@
       </c>
       <c r="C15" s="2">
         <v>9.9688499999999996E-3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1429 metaData with empty values imported (#1507)
* fix

* refactoring integration tests

* integration test added
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Presentation.Tests/Data/IntegrationSample1.xlsx
+++ b/tests/OSPSuite.Presentation.Tests/Data/IntegrationSample1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgiosDaskalakis\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.Presentation.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D00D0C-162C-4DDC-8FD2-3615B040848C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF71806C-E154-417A-B41D-9B12908A82EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="2358" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>time  [h]</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Molecular Weight</t>
+  </si>
+  <si>
+    <t>Dose</t>
   </si>
 </sst>
 </file>
@@ -389,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -401,7 +404,7 @@
     <col min="2" max="3" width="12.3125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,8 +417,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -429,7 +435,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>0.24454149999999999</v>
       </c>
@@ -443,7 +449,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>0.50655019999999995</v>
       </c>
@@ -457,7 +463,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
         <v>0.76855899999999999</v>
       </c>
@@ -471,7 +477,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>0.9956332</v>
       </c>
@@ -485,7 +491,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
         <v>1.2576419999999999</v>
       </c>
@@ -499,7 +505,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>1.502183</v>
       </c>
@@ -513,7 +519,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>1.764192</v>
       </c>
@@ -527,7 +533,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
         <v>2.008734</v>
       </c>
@@ -541,7 +547,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>3.0043669999999998</v>
       </c>
@@ -555,7 +561,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>4</v>
       </c>
@@ -569,7 +575,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>6.0087339999999996</v>
       </c>
@@ -583,7 +589,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>8</v>
       </c>
@@ -597,7 +603,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
         <v>12.017469999999999</v>
       </c>

</xml_diff>